<commit_message>
se cambia los nombres de los agentes.
</commit_message>
<xml_diff>
--- a/Documentacion/UAT-METRICAS.xlsx
+++ b/Documentacion/UAT-METRICAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="10005" windowHeight="10005" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="10005" windowHeight="10005" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Coca-Datos" sheetId="1" r:id="rId1"/>
@@ -142,19 +142,7 @@
     <t>possible points</t>
   </si>
   <si>
-    <t>Juan perez</t>
-  </si>
-  <si>
     <t>octubre</t>
-  </si>
-  <si>
-    <t>Jose Flores</t>
-  </si>
-  <si>
-    <t>Total Romualdo</t>
-  </si>
-  <si>
-    <t>Lorena García</t>
   </si>
   <si>
     <t>Total campaña Coca-Cola</t>
@@ -203,6 +191,18 @@
   </si>
   <si>
     <t>Augusto Arribalzaga</t>
+  </si>
+  <si>
+    <t>acoca1</t>
+  </si>
+  <si>
+    <t>acoca2</t>
+  </si>
+  <si>
+    <t>acoca3</t>
+  </si>
+  <si>
+    <t>Total scoca1</t>
   </si>
 </sst>
 </file>
@@ -2753,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2784,10 +2784,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C2" s="6">
         <f>SUM('Coca-Datos'!D2:D32)</f>
@@ -2804,10 +2804,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6">
         <f>SUM('Coca-Datos'!D33:D63)</f>
@@ -2825,7 +2825,7 @@
     <row r="4" spans="1:6">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="7">
         <f>SUM(C2:C3)</f>
@@ -2840,15 +2840,15 @@
         <v>1834</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="8">
         <f>SUM('Coca-Datos'!D64:D94)</f>
@@ -2880,7 +2880,7 @@
         <v>2731</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2906,28 +2906,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -5527,7 +5527,7 @@
         <v>105</v>
       </c>
       <c r="F88" s="13">
-        <f t="shared" ref="F86:F125" si="0">ROUNDDOWN(((B88+D88)-(A88+C88))*24,0)</f>
+        <f t="shared" ref="F88:F123" si="0">ROUNDDOWN(((B88+D88)-(A88+C88))*24,0)</f>
         <v>6</v>
       </c>
       <c r="G88" s="10">
@@ -6836,7 +6836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -6853,18 +6853,18 @@
         <v>36</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="6">
         <v>9</v>
@@ -6880,7 +6880,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B3" s="6">
         <v>9</v>
@@ -6896,7 +6896,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -6912,7 +6912,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B5" s="6">
         <v>9</v>

</xml_diff>

<commit_message>
se agrega la campaña 2 (clarín)
</commit_message>
<xml_diff>
--- a/Documentacion/UAT-METRICAS.xlsx
+++ b/Documentacion/UAT-METRICAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="10005" windowHeight="10005" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="10005" windowHeight="10005" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Coca-Datos" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>DOCKET</t>
   </si>
@@ -163,16 +163,7 @@
     <t>agente</t>
   </si>
   <si>
-    <t>Pablo Cohen</t>
-  </si>
-  <si>
     <t>AUX_TM</t>
-  </si>
-  <si>
-    <t>Damian Molinari</t>
-  </si>
-  <si>
-    <t>Martin Colinas</t>
   </si>
   <si>
     <t>Tiempo logueado</t>
@@ -190,9 +181,6 @@
     <t>HS_PRODUCTIVAS</t>
   </si>
   <si>
-    <t>Augusto Arribalzaga</t>
-  </si>
-  <si>
     <t>acoca1</t>
   </si>
   <si>
@@ -204,6 +192,36 @@
   <si>
     <t>Total scoca1</t>
   </si>
+  <si>
+    <t>aclarin1</t>
+  </si>
+  <si>
+    <t>aclarin2</t>
+  </si>
+  <si>
+    <t>aclarin3</t>
+  </si>
+  <si>
+    <t>aclarin4</t>
+  </si>
+  <si>
+    <t>Total sclarin1</t>
+  </si>
+  <si>
+    <t>Total campaña Clarín</t>
+  </si>
+  <si>
+    <t>AVG_TALK_TM</t>
+  </si>
+  <si>
+    <t>AVAIL_TM</t>
+  </si>
+  <si>
+    <t>IN_CALL</t>
+  </si>
+  <si>
+    <t>QUANTITY_OF_CALLS</t>
+  </si>
 </sst>
 </file>
 
@@ -214,7 +232,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -375,8 +393,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -572,6 +596,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -748,7 +778,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -791,6 +821,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2753,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2784,7 +2820,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>41</v>
@@ -2804,7 +2840,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>41</v>
@@ -2840,12 +2876,12 @@
         <v>1834</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>41</v>
@@ -2890,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I169"/>
+  <dimension ref="A1:K169"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2902,9 +2938,11 @@
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -2921,16 +2959,22 @@
         <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="11">
         <v>40452</v>
       </c>
@@ -2959,8 +3003,14 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>110</v>
+      </c>
+      <c r="K2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="11">
         <v>40453</v>
       </c>
@@ -2989,8 +3039,14 @@
       <c r="I3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>188</v>
+      </c>
+      <c r="K3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="11">
         <v>40454</v>
       </c>
@@ -3019,8 +3075,14 @@
       <c r="I4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>191</v>
+      </c>
+      <c r="K4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="11">
         <v>40455</v>
       </c>
@@ -3049,8 +3111,14 @@
       <c r="I5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>198</v>
+      </c>
+      <c r="K5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="11">
         <v>40456</v>
       </c>
@@ -3079,8 +3147,14 @@
       <c r="I6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>163</v>
+      </c>
+      <c r="K6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="11">
         <v>40457</v>
       </c>
@@ -3109,8 +3183,14 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>130</v>
+      </c>
+      <c r="K7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="11">
         <v>40458</v>
       </c>
@@ -3139,8 +3219,14 @@
       <c r="I8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>199</v>
+      </c>
+      <c r="K8">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="11">
         <v>40459</v>
       </c>
@@ -3169,8 +3255,14 @@
       <c r="I9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>144</v>
+      </c>
+      <c r="K9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="11">
         <v>40460</v>
       </c>
@@ -3199,8 +3291,14 @@
       <c r="I10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>104</v>
+      </c>
+      <c r="K10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="11">
         <v>40461</v>
       </c>
@@ -3229,8 +3327,14 @@
       <c r="I11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <v>162</v>
+      </c>
+      <c r="K11">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="11">
         <v>40462</v>
       </c>
@@ -3259,8 +3363,14 @@
       <c r="I12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12">
+        <v>120</v>
+      </c>
+      <c r="K12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="11">
         <v>40463</v>
       </c>
@@ -3289,8 +3399,14 @@
       <c r="I13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13">
+        <v>157</v>
+      </c>
+      <c r="K13">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="11">
         <v>40464</v>
       </c>
@@ -3319,8 +3435,14 @@
       <c r="I14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14">
+        <v>111</v>
+      </c>
+      <c r="K14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="11">
         <v>40465</v>
       </c>
@@ -3349,8 +3471,14 @@
       <c r="I15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15">
+        <v>183</v>
+      </c>
+      <c r="K15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="11">
         <v>40466</v>
       </c>
@@ -3379,8 +3507,14 @@
       <c r="I16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <v>140</v>
+      </c>
+      <c r="K16">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="11">
         <v>40467</v>
       </c>
@@ -3409,8 +3543,14 @@
       <c r="I17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <v>105</v>
+      </c>
+      <c r="K17">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="11">
         <v>40468</v>
       </c>
@@ -3439,8 +3579,14 @@
       <c r="I18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <v>113</v>
+      </c>
+      <c r="K18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="11">
         <v>40469</v>
       </c>
@@ -3469,8 +3615,14 @@
       <c r="I19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19">
+        <v>118</v>
+      </c>
+      <c r="K19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="11">
         <v>40470</v>
       </c>
@@ -3499,8 +3651,14 @@
       <c r="I20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20">
+        <v>152</v>
+      </c>
+      <c r="K20">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="11">
         <v>40471</v>
       </c>
@@ -3529,8 +3687,14 @@
       <c r="I21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21">
+        <v>188</v>
+      </c>
+      <c r="K21">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="11">
         <v>40472</v>
       </c>
@@ -3559,8 +3723,14 @@
       <c r="I22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22">
+        <v>132</v>
+      </c>
+      <c r="K22">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="11">
         <v>40473</v>
       </c>
@@ -3589,8 +3759,14 @@
       <c r="I23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23">
+        <v>143</v>
+      </c>
+      <c r="K23">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="11">
         <v>40474</v>
       </c>
@@ -3619,8 +3795,14 @@
       <c r="I24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24">
+        <v>138</v>
+      </c>
+      <c r="K24">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="11">
         <v>40475</v>
       </c>
@@ -3649,8 +3831,14 @@
       <c r="I25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25">
+        <v>158</v>
+      </c>
+      <c r="K25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="11">
         <v>40476</v>
       </c>
@@ -3679,8 +3867,14 @@
       <c r="I26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26">
+        <v>124</v>
+      </c>
+      <c r="K26">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="11">
         <v>40477</v>
       </c>
@@ -3709,8 +3903,14 @@
       <c r="I27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27">
+        <v>116</v>
+      </c>
+      <c r="K27">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="11">
         <v>40478</v>
       </c>
@@ -3739,8 +3939,14 @@
       <c r="I28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28">
+        <v>128</v>
+      </c>
+      <c r="K28">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="11">
         <v>40479</v>
       </c>
@@ -3769,8 +3975,14 @@
       <c r="I29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29">
+        <v>108</v>
+      </c>
+      <c r="K29">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="11">
         <v>40480</v>
       </c>
@@ -3799,8 +4011,14 @@
       <c r="I30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30">
+        <v>170</v>
+      </c>
+      <c r="K30">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="11">
         <v>40481</v>
       </c>
@@ -3829,8 +4047,14 @@
       <c r="I31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31">
+        <v>119</v>
+      </c>
+      <c r="K31">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="11">
         <v>40482</v>
       </c>
@@ -3859,8 +4083,14 @@
       <c r="I32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32">
+        <v>125</v>
+      </c>
+      <c r="K32">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="14">
         <v>40452</v>
       </c>
@@ -3889,8 +4119,14 @@
       <c r="I33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33">
+        <v>138</v>
+      </c>
+      <c r="K33">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="14">
         <v>40453</v>
       </c>
@@ -3919,8 +4155,14 @@
       <c r="I34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34">
+        <v>113</v>
+      </c>
+      <c r="K34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="14">
         <v>40454</v>
       </c>
@@ -3949,8 +4191,14 @@
       <c r="I35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35">
+        <v>129</v>
+      </c>
+      <c r="K35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="14">
         <v>40455</v>
       </c>
@@ -3979,8 +4227,14 @@
       <c r="I36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36">
+        <v>153</v>
+      </c>
+      <c r="K36">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="14">
         <v>40456</v>
       </c>
@@ -4009,8 +4263,14 @@
       <c r="I37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37">
+        <v>100</v>
+      </c>
+      <c r="K37">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="14">
         <v>40457</v>
       </c>
@@ -4039,8 +4299,14 @@
       <c r="I38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38">
+        <v>172</v>
+      </c>
+      <c r="K38">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="14">
         <v>40458</v>
       </c>
@@ -4069,8 +4335,14 @@
       <c r="I39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39">
+        <v>163</v>
+      </c>
+      <c r="K39">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="14">
         <v>40459</v>
       </c>
@@ -4099,8 +4371,14 @@
       <c r="I40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40">
+        <v>101</v>
+      </c>
+      <c r="K40">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="14">
         <v>40460</v>
       </c>
@@ -4129,8 +4407,14 @@
       <c r="I41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41">
+        <v>195</v>
+      </c>
+      <c r="K41">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="14">
         <v>40461</v>
       </c>
@@ -4159,8 +4443,14 @@
       <c r="I42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42">
+        <v>191</v>
+      </c>
+      <c r="K42">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="14">
         <v>40462</v>
       </c>
@@ -4189,8 +4479,14 @@
       <c r="I43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43">
+        <v>155</v>
+      </c>
+      <c r="K43">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="14">
         <v>40463</v>
       </c>
@@ -4219,8 +4515,14 @@
       <c r="I44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44">
+        <v>158</v>
+      </c>
+      <c r="K44">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="14">
         <v>40464</v>
       </c>
@@ -4249,8 +4551,14 @@
       <c r="I45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45">
+        <v>100</v>
+      </c>
+      <c r="K45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="14">
         <v>40465</v>
       </c>
@@ -4279,8 +4587,14 @@
       <c r="I46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46">
+        <v>185</v>
+      </c>
+      <c r="K46">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="14">
         <v>40466</v>
       </c>
@@ -4309,8 +4623,14 @@
       <c r="I47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47">
+        <v>165</v>
+      </c>
+      <c r="K47">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="14">
         <v>40467</v>
       </c>
@@ -4339,8 +4659,14 @@
       <c r="I48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48">
+        <v>107</v>
+      </c>
+      <c r="K48">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="14">
         <v>40468</v>
       </c>
@@ -4369,8 +4695,14 @@
       <c r="I49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49">
+        <v>159</v>
+      </c>
+      <c r="K49">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="14">
         <v>40469</v>
       </c>
@@ -4399,8 +4731,14 @@
       <c r="I50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50">
+        <v>173</v>
+      </c>
+      <c r="K50">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="14">
         <v>40470</v>
       </c>
@@ -4429,8 +4767,14 @@
       <c r="I51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51">
+        <v>162</v>
+      </c>
+      <c r="K51">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="14">
         <v>40471</v>
       </c>
@@ -4459,8 +4803,14 @@
       <c r="I52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52">
+        <v>147</v>
+      </c>
+      <c r="K52">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="14">
         <v>40472</v>
       </c>
@@ -4489,8 +4839,14 @@
       <c r="I53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53">
+        <v>105</v>
+      </c>
+      <c r="K53">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="14">
         <v>40473</v>
       </c>
@@ -4519,8 +4875,14 @@
       <c r="I54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54">
+        <v>183</v>
+      </c>
+      <c r="K54">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="14">
         <v>40474</v>
       </c>
@@ -4549,8 +4911,14 @@
       <c r="I55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55">
+        <v>153</v>
+      </c>
+      <c r="K55">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="14">
         <v>40475</v>
       </c>
@@ -4579,8 +4947,14 @@
       <c r="I56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56">
+        <v>112</v>
+      </c>
+      <c r="K56">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="14">
         <v>40476</v>
       </c>
@@ -4609,8 +4983,14 @@
       <c r="I57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57">
+        <v>128</v>
+      </c>
+      <c r="K57">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="14">
         <v>40477</v>
       </c>
@@ -4639,8 +5019,14 @@
       <c r="I58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58">
+        <v>172</v>
+      </c>
+      <c r="K58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="14">
         <v>40478</v>
       </c>
@@ -4669,8 +5055,14 @@
       <c r="I59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59">
+        <v>176</v>
+      </c>
+      <c r="K59">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="14">
         <v>40479</v>
       </c>
@@ -4699,8 +5091,14 @@
       <c r="I60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60">
+        <v>161</v>
+      </c>
+      <c r="K60">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="14">
         <v>40480</v>
       </c>
@@ -4729,8 +5127,14 @@
       <c r="I61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61">
+        <v>101</v>
+      </c>
+      <c r="K61">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="14">
         <v>40481</v>
       </c>
@@ -4759,8 +5163,14 @@
       <c r="I62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62">
+        <v>109</v>
+      </c>
+      <c r="K62">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="14">
         <v>40482</v>
       </c>
@@ -4789,8 +5199,14 @@
       <c r="I63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63">
+        <v>161</v>
+      </c>
+      <c r="K63">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="14">
         <v>40452</v>
       </c>
@@ -4819,8 +5235,14 @@
       <c r="I64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64">
+        <v>106</v>
+      </c>
+      <c r="K64">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="14">
         <v>40453</v>
       </c>
@@ -4849,8 +5271,14 @@
       <c r="I65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="J65">
+        <v>157</v>
+      </c>
+      <c r="K65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="14">
         <v>40454</v>
       </c>
@@ -4879,8 +5307,14 @@
       <c r="I66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="J66">
+        <v>186</v>
+      </c>
+      <c r="K66">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="14">
         <v>40455</v>
       </c>
@@ -4909,8 +5343,14 @@
       <c r="I67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="J67">
+        <v>107</v>
+      </c>
+      <c r="K67">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" s="14">
         <v>40456</v>
       </c>
@@ -4939,8 +5379,14 @@
       <c r="I68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="J68">
+        <v>129</v>
+      </c>
+      <c r="K68">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" s="14">
         <v>40457</v>
       </c>
@@ -4969,8 +5415,14 @@
       <c r="I69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="J69">
+        <v>168</v>
+      </c>
+      <c r="K69">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="14">
         <v>40458</v>
       </c>
@@ -4999,8 +5451,14 @@
       <c r="I70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="J70">
+        <v>164</v>
+      </c>
+      <c r="K70">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" s="14">
         <v>40459</v>
       </c>
@@ -5029,8 +5487,14 @@
       <c r="I71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="J71">
+        <v>187</v>
+      </c>
+      <c r="K71">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="14">
         <v>40460</v>
       </c>
@@ -5059,8 +5523,14 @@
       <c r="I72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="J72">
+        <v>154</v>
+      </c>
+      <c r="K72">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="14">
         <v>40461</v>
       </c>
@@ -5089,8 +5559,14 @@
       <c r="I73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="J73">
+        <v>104</v>
+      </c>
+      <c r="K73">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="14">
         <v>40462</v>
       </c>
@@ -5119,8 +5595,14 @@
       <c r="I74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="J74">
+        <v>151</v>
+      </c>
+      <c r="K74">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="14">
         <v>40463</v>
       </c>
@@ -5149,8 +5631,14 @@
       <c r="I75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="J75">
+        <v>141</v>
+      </c>
+      <c r="K75">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="14">
         <v>40464</v>
       </c>
@@ -5179,8 +5667,14 @@
       <c r="I76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="J76">
+        <v>128</v>
+      </c>
+      <c r="K76">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="14">
         <v>40465</v>
       </c>
@@ -5209,8 +5703,14 @@
       <c r="I77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="J77">
+        <v>178</v>
+      </c>
+      <c r="K77">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="14">
         <v>40466</v>
       </c>
@@ -5239,8 +5739,14 @@
       <c r="I78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78">
+        <v>115</v>
+      </c>
+      <c r="K78">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="14">
         <v>40467</v>
       </c>
@@ -5269,8 +5775,14 @@
       <c r="I79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79">
+        <v>108</v>
+      </c>
+      <c r="K79">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="14">
         <v>40468</v>
       </c>
@@ -5299,8 +5811,14 @@
       <c r="I80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80">
+        <v>130</v>
+      </c>
+      <c r="K80">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" s="14">
         <v>40469</v>
       </c>
@@ -5329,8 +5847,14 @@
       <c r="I81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81">
+        <v>176</v>
+      </c>
+      <c r="K81">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" s="14">
         <v>40470</v>
       </c>
@@ -5359,8 +5883,14 @@
       <c r="I82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82">
+        <v>169</v>
+      </c>
+      <c r="K82">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="14">
         <v>40471</v>
       </c>
@@ -5389,8 +5919,14 @@
       <c r="I83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83">
+        <v>152</v>
+      </c>
+      <c r="K83">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="14">
         <v>40472</v>
       </c>
@@ -5419,8 +5955,14 @@
       <c r="I84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84">
+        <v>186</v>
+      </c>
+      <c r="K84">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" s="14">
         <v>40473</v>
       </c>
@@ -5449,8 +5991,14 @@
       <c r="I85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85">
+        <v>187</v>
+      </c>
+      <c r="K85">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" s="14">
         <v>40474</v>
       </c>
@@ -5479,8 +6027,14 @@
       <c r="I86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86">
+        <v>143</v>
+      </c>
+      <c r="K86">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" s="14">
         <v>40475</v>
       </c>
@@ -5509,8 +6063,14 @@
       <c r="I87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87">
+        <v>156</v>
+      </c>
+      <c r="K87">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" s="14">
         <v>40476</v>
       </c>
@@ -5539,8 +6099,14 @@
       <c r="I88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88">
+        <v>191</v>
+      </c>
+      <c r="K88">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" s="14">
         <v>40477</v>
       </c>
@@ -5569,8 +6135,14 @@
       <c r="I89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89">
+        <v>107</v>
+      </c>
+      <c r="K89">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" s="14">
         <v>40478</v>
       </c>
@@ -5599,8 +6171,14 @@
       <c r="I90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90">
+        <v>103</v>
+      </c>
+      <c r="K90">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" s="14">
         <v>40479</v>
       </c>
@@ -5629,8 +6207,14 @@
       <c r="I91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91">
+        <v>182</v>
+      </c>
+      <c r="K91">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" s="14">
         <v>40480</v>
       </c>
@@ -5659,8 +6243,14 @@
       <c r="I92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="J92">
+        <v>147</v>
+      </c>
+      <c r="K92">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" s="14">
         <v>40481</v>
       </c>
@@ -5689,8 +6279,14 @@
       <c r="I93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="J93">
+        <v>187</v>
+      </c>
+      <c r="K93">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" s="14">
         <v>40482</v>
       </c>
@@ -5719,8 +6315,14 @@
       <c r="I94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="J94">
+        <v>195</v>
+      </c>
+      <c r="K94">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" s="14">
         <v>40452</v>
       </c>
@@ -5749,8 +6351,14 @@
       <c r="I95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="J95">
+        <v>116</v>
+      </c>
+      <c r="K95">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" s="14">
         <v>40453</v>
       </c>
@@ -5779,8 +6387,14 @@
       <c r="I96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="J96">
+        <v>146</v>
+      </c>
+      <c r="K96">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" s="14">
         <v>40454</v>
       </c>
@@ -5809,8 +6423,14 @@
       <c r="I97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="J97">
+        <v>122</v>
+      </c>
+      <c r="K97">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" s="14">
         <v>40455</v>
       </c>
@@ -5839,8 +6459,14 @@
       <c r="I98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="J98">
+        <v>174</v>
+      </c>
+      <c r="K98">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" s="14">
         <v>40456</v>
       </c>
@@ -5869,8 +6495,14 @@
       <c r="I99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:9">
+      <c r="J99">
+        <v>122</v>
+      </c>
+      <c r="K99">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" s="14">
         <v>40457</v>
       </c>
@@ -5899,8 +6531,14 @@
       <c r="I100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="J100">
+        <v>176</v>
+      </c>
+      <c r="K100">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101" s="14">
         <v>40458</v>
       </c>
@@ -5929,8 +6567,14 @@
       <c r="I101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:9">
+      <c r="J101">
+        <v>196</v>
+      </c>
+      <c r="K101">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" s="14">
         <v>40459</v>
       </c>
@@ -5959,8 +6603,14 @@
       <c r="I102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="J102">
+        <v>187</v>
+      </c>
+      <c r="K102">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" s="14">
         <v>40460</v>
       </c>
@@ -5989,8 +6639,14 @@
       <c r="I103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:9">
+      <c r="J103">
+        <v>175</v>
+      </c>
+      <c r="K103">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" s="14">
         <v>40461</v>
       </c>
@@ -6019,8 +6675,14 @@
       <c r="I104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:9">
+      <c r="J104">
+        <v>171</v>
+      </c>
+      <c r="K104">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" s="14">
         <v>40462</v>
       </c>
@@ -6049,8 +6711,14 @@
       <c r="I105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:9">
+      <c r="J105">
+        <v>143</v>
+      </c>
+      <c r="K105">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" s="14">
         <v>40463</v>
       </c>
@@ -6079,8 +6747,14 @@
       <c r="I106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:9">
+      <c r="J106">
+        <v>123</v>
+      </c>
+      <c r="K106">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" s="14">
         <v>40464</v>
       </c>
@@ -6109,8 +6783,14 @@
       <c r="I107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="J107">
+        <v>129</v>
+      </c>
+      <c r="K107">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" s="14">
         <v>40465</v>
       </c>
@@ -6139,8 +6819,14 @@
       <c r="I108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="J108">
+        <v>196</v>
+      </c>
+      <c r="K108">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" s="14">
         <v>40466</v>
       </c>
@@ -6169,8 +6855,14 @@
       <c r="I109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:9">
+      <c r="J109">
+        <v>139</v>
+      </c>
+      <c r="K109">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110" s="14">
         <v>40467</v>
       </c>
@@ -6199,8 +6891,14 @@
       <c r="I110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:9">
+      <c r="J110">
+        <v>181</v>
+      </c>
+      <c r="K110">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111" s="14">
         <v>40468</v>
       </c>
@@ -6229,8 +6927,14 @@
       <c r="I111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="J111">
+        <v>176</v>
+      </c>
+      <c r="K111">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112" s="14">
         <v>40469</v>
       </c>
@@ -6259,8 +6963,14 @@
       <c r="I112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="J112">
+        <v>122</v>
+      </c>
+      <c r="K112">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113" s="14">
         <v>40470</v>
       </c>
@@ -6289,8 +6999,14 @@
       <c r="I113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="J113">
+        <v>131</v>
+      </c>
+      <c r="K113">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114" s="14">
         <v>40471</v>
       </c>
@@ -6319,8 +7035,14 @@
       <c r="I114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="J114">
+        <v>192</v>
+      </c>
+      <c r="K114">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115" s="14">
         <v>40472</v>
       </c>
@@ -6349,8 +7071,14 @@
       <c r="I115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="J115">
+        <v>100</v>
+      </c>
+      <c r="K115">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116" s="14">
         <v>40473</v>
       </c>
@@ -6379,8 +7107,14 @@
       <c r="I116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="J116">
+        <v>177</v>
+      </c>
+      <c r="K116">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" s="14">
         <v>40474</v>
       </c>
@@ -6409,8 +7143,14 @@
       <c r="I117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:9">
+      <c r="J117">
+        <v>192</v>
+      </c>
+      <c r="K117">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118" s="14">
         <v>40475</v>
       </c>
@@ -6439,8 +7179,14 @@
       <c r="I118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:9">
+      <c r="J118">
+        <v>197</v>
+      </c>
+      <c r="K118">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" s="14">
         <v>40476</v>
       </c>
@@ -6469,8 +7215,14 @@
       <c r="I119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:9">
+      <c r="J119">
+        <v>178</v>
+      </c>
+      <c r="K119">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120" s="14">
         <v>40477</v>
       </c>
@@ -6499,8 +7251,14 @@
       <c r="I120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:9">
+      <c r="J120">
+        <v>124</v>
+      </c>
+      <c r="K120">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121" s="14">
         <v>40478</v>
       </c>
@@ -6529,8 +7287,14 @@
       <c r="I121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="J121">
+        <v>123</v>
+      </c>
+      <c r="K121">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" s="14">
         <v>40479</v>
       </c>
@@ -6559,8 +7323,14 @@
       <c r="I122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:9">
+      <c r="J122">
+        <v>175</v>
+      </c>
+      <c r="K122">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" s="14">
         <v>40480</v>
       </c>
@@ -6589,8 +7359,14 @@
       <c r="I123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="J123">
+        <v>157</v>
+      </c>
+      <c r="K123">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" s="14">
         <v>40481</v>
       </c>
@@ -6619,8 +7395,14 @@
       <c r="I124">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="J124">
+        <v>173</v>
+      </c>
+      <c r="K124">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125" s="14">
         <v>40482</v>
       </c>
@@ -6649,18 +7431,24 @@
       <c r="I125">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:9">
+      <c r="J125">
+        <v>125</v>
+      </c>
+      <c r="K125">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="C126" s="12"/>
       <c r="D126" s="12"/>
       <c r="F126" s="13"/>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:11">
       <c r="C127" s="12"/>
       <c r="D127" s="12"/>
       <c r="F127" s="13"/>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:11">
       <c r="C128" s="12"/>
       <c r="D128" s="12"/>
       <c r="F128" s="13"/>
@@ -6834,99 +7622,335 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="6">
-        <v>9</v>
+        <v>58</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="6">
-        <f>(SUMIF('Clarin-Datos'!F2:F32,"&gt;0",'Clarin-Datos'!I2:I32)*B2+SUM('Clarin-Datos'!H2:H32))</f>
-        <v>241</v>
-      </c>
-      <c r="D2" s="17">
-        <f>C2*60-SUM('Clarin-Datos'!G2:G32)</f>
-        <v>7435</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6">
+        <f>(SUMIF('Clarin-Datos'!F2:F32,"&gt;0",'Clarin-Datos'!I2:I32)*C2+SUM('Clarin-Datos'!H2:H32))</f>
+        <v>199</v>
+      </c>
+      <c r="E2" s="17">
+        <f>D2*60-SUM('Clarin-Datos'!G2:G32)</f>
+        <v>4915</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(
+'Clarin-Datos'!J2*60/'Clarin-Datos'!K2,
+'Clarin-Datos'!J3*60/'Clarin-Datos'!K3,
+'Clarin-Datos'!J4*60/'Clarin-Datos'!K4,
+'Clarin-Datos'!J5*60/'Clarin-Datos'!K5,
+'Clarin-Datos'!J6*60/'Clarin-Datos'!K6,
+'Clarin-Datos'!J7*60/'Clarin-Datos'!K7,
+'Clarin-Datos'!J8*60/'Clarin-Datos'!K8,
+'Clarin-Datos'!J9*60/'Clarin-Datos'!K9,
+'Clarin-Datos'!J10*60/'Clarin-Datos'!K10,
+'Clarin-Datos'!J11*60/'Clarin-Datos'!K11,
+'Clarin-Datos'!J12*60/'Clarin-Datos'!K12,
+'Clarin-Datos'!J13*60/'Clarin-Datos'!K13,
+'Clarin-Datos'!J14*60/'Clarin-Datos'!K14,
+'Clarin-Datos'!J15*60/'Clarin-Datos'!K15,
+'Clarin-Datos'!J16*60/'Clarin-Datos'!K16,
+'Clarin-Datos'!J17*60/'Clarin-Datos'!K17,
+'Clarin-Datos'!J18*60/'Clarin-Datos'!K18,
+'Clarin-Datos'!J19*60/'Clarin-Datos'!K19,
+'Clarin-Datos'!J20*60/'Clarin-Datos'!K20,
+'Clarin-Datos'!J21*60/'Clarin-Datos'!K21,
+'Clarin-Datos'!J22*60/'Clarin-Datos'!K22,
+'Clarin-Datos'!J23*60/'Clarin-Datos'!K23,
+'Clarin-Datos'!J24*60/'Clarin-Datos'!K24,
+'Clarin-Datos'!J25*60/'Clarin-Datos'!K25,
+'Clarin-Datos'!J26*60/'Clarin-Datos'!K26,
+'Clarin-Datos'!J27*60/'Clarin-Datos'!K27,
+'Clarin-Datos'!J28*60/'Clarin-Datos'!K28,
+'Clarin-Datos'!J29*60/'Clarin-Datos'!K29,
+'Clarin-Datos'!J30*60/'Clarin-Datos'!K30,
+'Clarin-Datos'!J31*60/'Clarin-Datos'!K31,
+'Clarin-Datos'!J32*60/'Clarin-Datos'!K32)</f>
+        <v>140.26348022085023</v>
+      </c>
+      <c r="G2" s="18">
+        <f>SUM('Clarin-Datos'!J2:J32)</f>
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="6">
-        <v>9</v>
+        <v>59</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C3" s="6">
-        <f>SUMIF('Clarin-Datos'!F33:F63,"&gt;0",'Clarin-Datos'!I33:I63)*B3+SUM('Clarin-Datos'!H33:H63)</f>
-        <v>243</v>
-      </c>
-      <c r="D3" s="17">
-        <f>C3*60-SUM('Clarin-Datos'!G33:G63)</f>
-        <v>7578</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="6">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6">
-        <f>SUMIF('Clarin-Datos'!F64:F94,"&gt;0",'Clarin-Datos'!I64:I94)*B4+SUM('Clarin-Datos'!H64:H94)</f>
-        <v>245</v>
-      </c>
-      <c r="D4" s="17">
-        <f>C4*60-SUM('Clarin-Datos'!G64:G94)</f>
-        <v>7631</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6">
+        <f>SUMIF('Clarin-Datos'!F33:F63,"&gt;0",'Clarin-Datos'!I33:I63)*C3+SUM('Clarin-Datos'!H33:H63)</f>
+        <v>201</v>
+      </c>
+      <c r="E3" s="17">
+        <f>D3*60-SUM('Clarin-Datos'!G33:G63)</f>
+        <v>5058</v>
+      </c>
+      <c r="F3" s="18">
+        <f>AVERAGE(
+'Clarin-Datos'!J33*60/'Clarin-Datos'!K33,
+'Clarin-Datos'!J34*60/'Clarin-Datos'!K34,
+'Clarin-Datos'!J35*60/'Clarin-Datos'!K35,
+'Clarin-Datos'!J36*60/'Clarin-Datos'!K36,
+'Clarin-Datos'!J37*60/'Clarin-Datos'!K37,
+'Clarin-Datos'!J38*60/'Clarin-Datos'!K38,
+'Clarin-Datos'!J39*60/'Clarin-Datos'!K39,
+'Clarin-Datos'!J40*60/'Clarin-Datos'!K40,
+'Clarin-Datos'!J41*60/'Clarin-Datos'!K41,
+'Clarin-Datos'!J42*60/'Clarin-Datos'!K42,
+'Clarin-Datos'!J43*60/'Clarin-Datos'!K43,
+'Clarin-Datos'!J44*60/'Clarin-Datos'!K44,
+'Clarin-Datos'!J45*60/'Clarin-Datos'!K45,
+'Clarin-Datos'!J46*60/'Clarin-Datos'!K46,
+'Clarin-Datos'!J47*60/'Clarin-Datos'!K47,
+'Clarin-Datos'!J48*60/'Clarin-Datos'!K48,
+'Clarin-Datos'!J49*60/'Clarin-Datos'!K49,
+'Clarin-Datos'!J50*60/'Clarin-Datos'!K50,
+'Clarin-Datos'!J51*60/'Clarin-Datos'!K51,
+'Clarin-Datos'!J52*60/'Clarin-Datos'!K52,
+'Clarin-Datos'!J53*60/'Clarin-Datos'!K53,
+'Clarin-Datos'!J54*60/'Clarin-Datos'!K54,
+'Clarin-Datos'!J55*60/'Clarin-Datos'!K55,
+'Clarin-Datos'!J56*60/'Clarin-Datos'!K56,
+'Clarin-Datos'!J57*60/'Clarin-Datos'!K57,
+'Clarin-Datos'!J58*60/'Clarin-Datos'!K58,
+'Clarin-Datos'!J59*60/'Clarin-Datos'!K59,
+'Clarin-Datos'!J60*60/'Clarin-Datos'!K60,
+'Clarin-Datos'!J61*60/'Clarin-Datos'!K61,
+'Clarin-Datos'!J62*60/'Clarin-Datos'!K62,
+'Clarin-Datos'!J63*60/'Clarin-Datos'!K63)</f>
+        <v>153.62040260795868</v>
+      </c>
+      <c r="G3" s="18">
+        <f>SUM('Clarin-Datos'!J33:J63)</f>
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="7">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7">
+        <f>SUM(D2:D3)</f>
+        <v>400</v>
+      </c>
+      <c r="E4" s="7">
+        <f>SUM(E2:E3)</f>
+        <v>9973</v>
+      </c>
+      <c r="F4" s="7">
+        <f>AVERAGE(F2:F3)</f>
+        <v>146.94194141440445</v>
+      </c>
+      <c r="G4" s="7">
+        <f>SUM(G2:G3)</f>
+        <v>8964</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="6">
-        <v>9</v>
+        <v>60</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="6">
-        <f>SUMIF('Clarin-Datos'!F95:F125,"&gt;0",'Clarin-Datos'!I95:I125)*B5+SUM('Clarin-Datos'!H95:H125)</f>
-        <v>244</v>
-      </c>
-      <c r="D5" s="17">
-        <f>C5*60-SUM('Clarin-Datos'!G95:G125)</f>
-        <v>7341</v>
+        <v>7</v>
+      </c>
+      <c r="D5" s="6">
+        <f>SUMIF('Clarin-Datos'!F64:F94,"&gt;0",'Clarin-Datos'!I64:I94)*C5+SUM('Clarin-Datos'!H64:H94)</f>
+        <v>203</v>
+      </c>
+      <c r="E5" s="17">
+        <f>D5*60-SUM('Clarin-Datos'!G64:G94)</f>
+        <v>5111</v>
+      </c>
+      <c r="F5" s="18">
+        <f>AVERAGE(
+'Clarin-Datos'!J64*60/'Clarin-Datos'!K64,
+'Clarin-Datos'!J65*60/'Clarin-Datos'!K65,
+'Clarin-Datos'!J66*60/'Clarin-Datos'!K66,
+'Clarin-Datos'!J67*60/'Clarin-Datos'!K67,
+'Clarin-Datos'!J68*60/'Clarin-Datos'!K68,
+'Clarin-Datos'!J69*60/'Clarin-Datos'!K69,
+'Clarin-Datos'!J70*60/'Clarin-Datos'!K70,
+'Clarin-Datos'!J71*60/'Clarin-Datos'!K71,
+'Clarin-Datos'!J72*60/'Clarin-Datos'!K72,
+'Clarin-Datos'!J73*60/'Clarin-Datos'!K73,
+'Clarin-Datos'!J74*60/'Clarin-Datos'!K74,
+'Clarin-Datos'!J75*60/'Clarin-Datos'!K75,
+'Clarin-Datos'!J76*60/'Clarin-Datos'!K76,
+'Clarin-Datos'!J77*60/'Clarin-Datos'!K77,
+'Clarin-Datos'!J78*60/'Clarin-Datos'!K78,
+'Clarin-Datos'!J79*60/'Clarin-Datos'!K79,
+'Clarin-Datos'!J80*60/'Clarin-Datos'!K80,
+'Clarin-Datos'!J81*60/'Clarin-Datos'!K81,
+'Clarin-Datos'!J82*60/'Clarin-Datos'!K82,
+'Clarin-Datos'!J83*60/'Clarin-Datos'!K83,
+'Clarin-Datos'!J84*60/'Clarin-Datos'!K84,
+'Clarin-Datos'!J85*60/'Clarin-Datos'!K85,
+'Clarin-Datos'!J86*60/'Clarin-Datos'!K86,
+'Clarin-Datos'!J87*60/'Clarin-Datos'!K87,
+'Clarin-Datos'!J88*60/'Clarin-Datos'!K88,
+'Clarin-Datos'!J89*60/'Clarin-Datos'!K89,
+'Clarin-Datos'!J90*60/'Clarin-Datos'!K90,
+'Clarin-Datos'!J91*60/'Clarin-Datos'!K91,
+'Clarin-Datos'!J92*60/'Clarin-Datos'!K92,
+'Clarin-Datos'!J93*60/'Clarin-Datos'!K93,
+'Clarin-Datos'!J94*60/'Clarin-Datos'!K94)</f>
+        <v>163.69609088609747</v>
+      </c>
+      <c r="G5" s="18">
+        <f>SUM('Clarin-Datos'!J64:J94)</f>
+        <v>4694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="6">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <f>SUMIF('Clarin-Datos'!F95:F125,"&gt;0",'Clarin-Datos'!I95:I125)*C6+SUM('Clarin-Datos'!H95:H125)</f>
+        <v>202</v>
+      </c>
+      <c r="E6" s="17">
+        <f>D6*60-SUM('Clarin-Datos'!G95:G125)</f>
+        <v>4821</v>
+      </c>
+      <c r="F6" s="18">
+        <f>AVERAGE(
+'Clarin-Datos'!J95*60/'Clarin-Datos'!K95,
+'Clarin-Datos'!J96*60/'Clarin-Datos'!K96,
+'Clarin-Datos'!J97*60/'Clarin-Datos'!K97,
+'Clarin-Datos'!J98*60/'Clarin-Datos'!K98,
+'Clarin-Datos'!J99*60/'Clarin-Datos'!K99,
+'Clarin-Datos'!J100*60/'Clarin-Datos'!K100,
+'Clarin-Datos'!J101*60/'Clarin-Datos'!K101,
+'Clarin-Datos'!J102*60/'Clarin-Datos'!K102,
+'Clarin-Datos'!J103*60/'Clarin-Datos'!K103,
+'Clarin-Datos'!J104*60/'Clarin-Datos'!K104,
+'Clarin-Datos'!J105*60/'Clarin-Datos'!K105,
+'Clarin-Datos'!J106*60/'Clarin-Datos'!K106,
+'Clarin-Datos'!J107*60/'Clarin-Datos'!K107,
+'Clarin-Datos'!J108*60/'Clarin-Datos'!K108,
+'Clarin-Datos'!J109*60/'Clarin-Datos'!K109,
+'Clarin-Datos'!J110*60/'Clarin-Datos'!K110,
+'Clarin-Datos'!J111*60/'Clarin-Datos'!K111,
+'Clarin-Datos'!J112*60/'Clarin-Datos'!K112,
+'Clarin-Datos'!J113*60/'Clarin-Datos'!K113,
+'Clarin-Datos'!J114*60/'Clarin-Datos'!K114,
+'Clarin-Datos'!J115*60/'Clarin-Datos'!K115,
+'Clarin-Datos'!J116*60/'Clarin-Datos'!K116,
+'Clarin-Datos'!J117*60/'Clarin-Datos'!K117,
+'Clarin-Datos'!J118*60/'Clarin-Datos'!K118,
+'Clarin-Datos'!J119*60/'Clarin-Datos'!K119,
+'Clarin-Datos'!J120*60/'Clarin-Datos'!K120,
+'Clarin-Datos'!J121*60/'Clarin-Datos'!K121,
+'Clarin-Datos'!J122*60/'Clarin-Datos'!K122,
+'Clarin-Datos'!J123*60/'Clarin-Datos'!K123,
+'Clarin-Datos'!J124*60/'Clarin-Datos'!K124,
+'Clarin-Datos'!J125*60/'Clarin-Datos'!K125)</f>
+        <v>154.35010069266909</v>
+      </c>
+      <c r="G6" s="18">
+        <f>SUM('Clarin-Datos'!J95:J125)</f>
+        <v>4838</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7">
+        <f>SUM(D4:D6)</f>
+        <v>805</v>
+      </c>
+      <c r="E7" s="19">
+        <f>SUM(E2,E3,E5,E6)</f>
+        <v>19905</v>
+      </c>
+      <c r="F7" s="7">
+        <f>AVERAGE(F2,F3,F5,F6)</f>
+        <v>152.98251860189387</v>
+      </c>
+      <c r="G7" s="7">
+        <f>SUM(G4:G6)</f>
+        <v>18496</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>